<commit_message>
Comment => Annotation in XLSX
</commit_message>
<xml_diff>
--- a/painting/E130.xlsx
+++ b/painting/E130.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbaker/github/dcmi/dcap/painting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4627D0D5-E34C-6847-84C3-AACF4822F007}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAD2687-A3F6-CE4C-8111-DE59B23E2AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="-28340" windowWidth="51120" windowHeight="28340" xr2:uid="{AAAF9636-5162-F145-914D-17D4807C7D56}"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{AAAF9636-5162-F145-914D-17D4807C7D56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Cardinality</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>painting</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Value_type</t>
+  </si>
+  <si>
+    <t>Annotation</t>
   </si>
 </sst>
 </file>
@@ -636,9 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97311BF0-D0F2-9B4E-808D-B118BF47D230}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="319" zoomScaleNormal="319" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="319" zoomScaleNormal="319" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -654,16 +652,16 @@
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>2</v>
@@ -672,123 +670,123 @@
         <v>1</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>